<commit_message>
Actualización de requisitos + pruebas
</commit_message>
<xml_diff>
--- a/Documentación/Requisitos.xlsx
+++ b/Documentación/Requisitos.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dwes\TFG_DAW\Documentación\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
   </bookViews>
@@ -14,12 +19,12 @@
     <definedName name="Título1">Requisitos_de_Proyecto[[#Headers],[Tarea]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Requisitos del Proyecto'!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>Tarea</t>
   </si>
@@ -130,12 +135,21 @@
   </si>
   <si>
     <t>Recordar contraseña</t>
+  </si>
+  <si>
+    <t>Los juegos se borran correctamente</t>
+  </si>
+  <si>
+    <t>Falta la comprobación del cod de verificación pero cumple su objetivo</t>
+  </si>
+  <si>
+    <t>KO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
@@ -144,7 +158,7 @@
     <numFmt numFmtId="168" formatCode="&quot;Finalizado&quot;;&quot;&quot;;&quot;Vencido&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;Finalizada&quot;;&quot;&quot;;&quot;Vencida&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
@@ -335,6 +349,7 @@
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Año del calendario" xfId="14"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="9" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Fecha" xfId="11"/>
     <cellStyle name="Finalizado o vencido" xfId="13"/>
@@ -344,9 +359,8 @@
     <cellStyle name="Moneda [0]" xfId="8" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Notas" xfId="10" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Porcentual" xfId="12" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Porcentaje" xfId="12" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
   </cellStyles>
@@ -578,7 +592,7 @@
         <xdr:cNvPr id="4" name="Lista de tareas pendientes anual" descr="Marcador de pestaña para el año">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -644,7 +658,7 @@
         <xdr:cNvPr id="3" name="Lista de tareas pendientes anual" descr="Forma de relleno de celda ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1018,18 +1032,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:J15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
@@ -1042,13 +1056,13 @@
     <col min="10" max="10" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="30" customHeight="1">
+    <row r="1" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I1" s="1">
         <f ca="1">YEAR(TODAY())</f>
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="84" customHeight="1">
+    <row r="2" spans="2:10" ht="84" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
@@ -1060,7 +1074,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="2:10" ht="30" customHeight="1">
+    <row r="3" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1089,7 +1103,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="30" customHeight="1">
+    <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
@@ -1119,7 +1133,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="30" customHeight="1">
+    <row r="5" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -1149,7 +1163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="30" customHeight="1">
+    <row r="6" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>19</v>
       </c>
@@ -1179,7 +1193,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1">
+    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -1207,7 +1221,7 @@
       </c>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="2:10" ht="30" customHeight="1">
+    <row r="8" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
@@ -1235,7 +1249,7 @@
       </c>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1">
+    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
@@ -1265,7 +1279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1">
+    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="6" t="s">
         <v>31</v>
       </c>
@@ -1273,7 +1287,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E10" s="7">
         <v>44550</v>
@@ -1282,16 +1296,20 @@
         <v>44713</v>
       </c>
       <c r="G10" s="2">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H10" s="4">
         <f ca="1">IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]="Completada",Requisitos_de_Proyecto[[#This Row],[Porcentaje completado]]=1),1,IF(ISBLANK(Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),-1,IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]&lt;&gt;"Completado",TODAY()&gt;Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),0,-1)))</f>
-        <v>-1</v>
-      </c>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1">
+    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
         <v>32</v>
       </c>
@@ -1321,7 +1339,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="30" customHeight="1">
+    <row r="12" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
@@ -1351,7 +1369,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1">
+    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
@@ -1374,10 +1392,14 @@
         <f ca="1">IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]="Completada",Requisitos_de_Proyecto[[#This Row],[Porcentaje completado]]=1),1,IF(ISBLANK(Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),-1,IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]&lt;&gt;"Completado",TODAY()&gt;Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),0,-1)))</f>
         <v>-1</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="I13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="14" spans="2:10" ht="30" customHeight="1">
+    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="6" t="s">
         <v>1</v>
       </c>
@@ -1403,7 +1425,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
     </row>
-    <row r="15" spans="2:10" ht="30" customHeight="1">
+    <row r="15" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="6" t="s">
         <v>2</v>
       </c>
@@ -1437,8 +1459,8 @@
   <conditionalFormatting sqref="G5:G15">
     <cfRule type="dataBar" priority="75">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1451,8 +1473,8 @@
   <conditionalFormatting sqref="G8:G11">
     <cfRule type="dataBar" priority="7">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1465,8 +1487,8 @@
   <conditionalFormatting sqref="G12:G15">
     <cfRule type="dataBar" priority="5">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1479,8 +1501,8 @@
   <conditionalFormatting sqref="G4">
     <cfRule type="dataBar" priority="3">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1493,8 +1515,8 @@
   <conditionalFormatting sqref="G4">
     <cfRule type="dataBar" priority="1">
       <dataBar>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>

</xml_diff>

<commit_message>
actualización de punto 4 doc + excel
</commit_message>
<xml_diff>
--- a/Documentación/Requisitos.xlsx
+++ b/Documentación/Requisitos.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DAW\TFG\Documentación\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7800"/>
   </bookViews>
@@ -19,7 +14,7 @@
     <definedName name="Título1">Requisitos_de_Proyecto[[#Headers],[Tarea]]</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Requisitos del Proyecto'!$3:$3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -137,9 +132,6 @@
     <t>Los juegos se borran correctamente</t>
   </si>
   <si>
-    <t>Falta la comprobación del cod de verificación pero cumple su objetivo</t>
-  </si>
-  <si>
     <t>KO</t>
   </si>
   <si>
@@ -174,12 +166,15 @@
   </si>
   <si>
     <t>Cabecera fija cuando el usuario hace scroll</t>
+  </si>
+  <si>
+    <t>todo OK, verificación de email, nickname y código</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
@@ -188,7 +183,7 @@
     <numFmt numFmtId="168" formatCode="&quot;Finalizado&quot;;&quot;&quot;;&quot;Vencido&quot;"/>
     <numFmt numFmtId="169" formatCode="&quot;Finalizada&quot;;&quot;&quot;;&quot;Vencida&quot;"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1" tint="4.9989318521683403E-2"/>
@@ -379,7 +374,6 @@
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Año del calendario" xfId="14"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="9" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Fecha" xfId="11"/>
     <cellStyle name="Finalizado o vencido" xfId="13"/>
@@ -389,8 +383,9 @@
     <cellStyle name="Moneda [0]" xfId="8" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Notas" xfId="10" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Porcentaje" xfId="12" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Porcentual" xfId="12" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
   </cellStyles>
@@ -622,7 +617,7 @@
         <xdr:cNvPr id="4" name="Lista de tareas pendientes anual" descr="Marcador de pestaña para el año">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -688,7 +683,7 @@
         <xdr:cNvPr id="3" name="Lista de tareas pendientes anual" descr="Forma de relleno de celda ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1063,18 +1058,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="30" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
@@ -1087,13 +1082,13 @@
     <col min="10" max="10" width="12.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="30" customHeight="1">
       <c r="I1" s="1">
         <f ca="1">YEAR(TODAY())</f>
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="84" customHeight="1">
       <c r="B2" s="8" t="s">
         <v>13</v>
       </c>
@@ -1105,7 +1100,7 @@
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
     </row>
-    <row r="3" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="30" customHeight="1">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1134,7 +1129,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="30" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>21</v>
       </c>
@@ -1164,7 +1159,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="30" customHeight="1">
       <c r="B5" t="s">
         <v>23</v>
       </c>
@@ -1194,7 +1189,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="30" customHeight="1">
       <c r="B6" t="s">
         <v>19</v>
       </c>
@@ -1224,7 +1219,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="30" customHeight="1">
       <c r="B7" t="s">
         <v>25</v>
       </c>
@@ -1252,7 +1247,7 @@
       </c>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="30" customHeight="1">
       <c r="B8" s="6" t="s">
         <v>27</v>
       </c>
@@ -1280,7 +1275,7 @@
       </c>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="30" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
@@ -1310,7 +1305,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="30" customHeight="1">
       <c r="B10" s="6" t="s">
         <v>31</v>
       </c>
@@ -1340,7 +1335,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="30" customHeight="1">
       <c r="B11" s="6" t="s">
         <v>32</v>
       </c>
@@ -1370,7 +1365,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="30" customHeight="1">
       <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
@@ -1400,15 +1395,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="30" customHeight="1">
       <c r="B13" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E13" s="7">
         <v>44550</v>
@@ -1417,22 +1412,22 @@
         <v>44713</v>
       </c>
       <c r="G13" s="2">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="H13" s="4">
         <f ca="1">IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]="Completada",Requisitos_de_Proyecto[[#This Row],[Porcentaje completado]]=1),1,IF(ISBLANK(Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),-1,IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]&lt;&gt;"Completado",TODAY()&gt;Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),0,-1)))</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="J13" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="30" customHeight="1">
+      <c r="B14" s="6" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
-        <v>39</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>6</v>
@@ -1454,15 +1449,15 @@
         <v>-1</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="30" customHeight="1">
       <c r="B15" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>4</v>
@@ -1484,15 +1479,15 @@
         <v>1</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="30" customHeight="1">
       <c r="B16" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>4</v>
@@ -1514,15 +1509,15 @@
         <v>1</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" ht="30" customHeight="1">
       <c r="B17" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>6</v>
@@ -1544,15 +1539,15 @@
         <v>1</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="30" customHeight="1">
       <c r="B18" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>6</v>
@@ -1574,13 +1569,13 @@
         <v>1</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J18" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="30" customHeight="1">
       <c r="B19" s="6" t="s">
         <v>2</v>
       </c>
@@ -1606,7 +1601,7 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
-    <row r="20" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="30" customHeight="1">
       <c r="B20" s="6" t="s">
         <v>1</v>
       </c>
@@ -1632,7 +1627,7 @@
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
-    <row r="21" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="30" customHeight="1">
       <c r="B21" s="6" t="s">
         <v>2</v>
       </c>
@@ -1666,8 +1661,8 @@
   <conditionalFormatting sqref="G5:G15">
     <cfRule type="dataBar" priority="87">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1680,8 +1675,8 @@
   <conditionalFormatting sqref="G8:G11">
     <cfRule type="dataBar" priority="19">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1694,8 +1689,8 @@
   <conditionalFormatting sqref="G12:G15">
     <cfRule type="dataBar" priority="17">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1708,8 +1703,8 @@
   <conditionalFormatting sqref="G4">
     <cfRule type="dataBar" priority="15">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1722,8 +1717,8 @@
   <conditionalFormatting sqref="G4">
     <cfRule type="dataBar" priority="13">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1736,8 +1731,8 @@
   <conditionalFormatting sqref="G16:G17">
     <cfRule type="dataBar" priority="11">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1750,8 +1745,8 @@
   <conditionalFormatting sqref="G16:G17">
     <cfRule type="dataBar" priority="9">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1764,8 +1759,8 @@
   <conditionalFormatting sqref="G18:G19">
     <cfRule type="dataBar" priority="7">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1778,8 +1773,8 @@
   <conditionalFormatting sqref="G18:G19">
     <cfRule type="dataBar" priority="5">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1792,8 +1787,8 @@
   <conditionalFormatting sqref="G20:G21">
     <cfRule type="dataBar" priority="3">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>
@@ -1806,8 +1801,8 @@
   <conditionalFormatting sqref="G20:G21">
     <cfRule type="dataBar" priority="1">
       <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
         <color theme="3" tint="0.39997558519241921"/>
       </dataBar>
       <extLst>

</xml_diff>

<commit_message>
docu excel + arreglo índice
</commit_message>
<xml_diff>
--- a/Documentación/Requisitos.xlsx
+++ b/Documentación/Requisitos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>Tarea</t>
   </si>
@@ -166,6 +166,12 @@
   </si>
   <si>
     <t xml:space="preserve">Resolver pequeños errores </t>
+  </si>
+  <si>
+    <t>Mostrar Contraseña</t>
+  </si>
+  <si>
+    <t>Muestra la contraseña de todos los formularios.</t>
   </si>
 </sst>
 </file>
@@ -614,7 +620,7 @@
         <xdr:cNvPr id="4" name="Lista de tareas pendientes anual" descr="Marcador de pestaña para el año">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{393B2DC2-9E53-4F1A-94BC-FD94F8128FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -680,7 +686,7 @@
         <xdr:cNvPr id="3" name="Lista de tareas pendientes anual" descr="Forma de relleno de celda ">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1062,8 +1068,8 @@
   </sheetPr>
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B9" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="30" customHeight="1"/>
@@ -1233,7 +1239,7 @@
         <v>44713</v>
       </c>
       <c r="G7" s="2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H7" s="4">
         <f ca="1">IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]="Completada",Requisitos_de_Proyecto[[#This Row],[Porcentaje completado]]=1),1,IF(ISBLANK(Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),-1,IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]&lt;&gt;"Completado",TODAY()&gt;Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),0,-1)))</f>
@@ -1261,7 +1267,7 @@
         <v>44713</v>
       </c>
       <c r="G8" s="2">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H8" s="4">
         <f ca="1">IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]="Completada",Requisitos_de_Proyecto[[#This Row],[Porcentaje completado]]=1),1,IF(ISBLANK(Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),-1,IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]&lt;&gt;"Completado",TODAY()&gt;Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),0,-1)))</f>
@@ -1574,13 +1580,13 @@
     </row>
     <row r="19" spans="2:10" ht="30" customHeight="1">
       <c r="B19" s="6" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E19" s="7">
         <v>44550</v>
@@ -1589,14 +1595,18 @@
         <v>44713</v>
       </c>
       <c r="G19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="4">
         <f ca="1">IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]="Completada",Requisitos_de_Proyecto[[#This Row],[Porcentaje completado]]=1),1,IF(ISBLANK(Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),-1,IF(AND(Requisitos_de_Proyecto[[#This Row],[Estado ]]&lt;&gt;"Completado",TODAY()&gt;Requisitos_de_Proyecto[[#This Row],[Fecha de entrega]]),0,-1)))</f>
-        <v>-1</v>
-      </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="2:10" ht="30" customHeight="1">
       <c r="B20" s="6" t="s">

</xml_diff>